<commit_message>
Improved script for reading from files
</commit_message>
<xml_diff>
--- a/test_metafile_2boxes.xlsx
+++ b/test_metafile_2boxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14145" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14145" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="thph12_metafile" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="229">
   <si>
     <t>tdtfile</t>
   </si>
@@ -648,18 +648,9 @@
     <t>!2017-08-16_10h52m.Subject THPH2.7</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>uv</t>
-  </si>
-  <si>
     <t>tick</t>
   </si>
   <si>
-    <t>distractors</t>
-  </si>
-  <si>
     <t>Dv1A</t>
   </si>
   <si>
@@ -703,6 +694,21 @@
   </si>
   <si>
     <t>Do2_</t>
+  </si>
+  <si>
+    <t>sig-blue</t>
+  </si>
+  <si>
+    <t>sig-uv</t>
+  </si>
+  <si>
+    <t>ttl-licks</t>
+  </si>
+  <si>
+    <t>ttl-distractors</t>
+  </si>
+  <si>
+    <t>ttl-distracted</t>
   </si>
 </sst>
 </file>
@@ -1271,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1319,22 +1325,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>17</v>
@@ -1375,22 +1381,22 @@
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -1428,22 +1434,22 @@
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -1481,22 +1487,22 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
@@ -1534,22 +1540,22 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -1587,22 +1593,22 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
@@ -1640,22 +1646,22 @@
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R7" s="2">
         <v>1</v>
@@ -1693,22 +1699,22 @@
         <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R8" s="2">
         <v>1</v>
@@ -1746,22 +1752,22 @@
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R9" s="2">
         <v>1</v>
@@ -1799,22 +1805,22 @@
         <v>0</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R10" s="2">
         <v>1</v>
@@ -1852,22 +1858,22 @@
         <v>0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R11" s="2">
         <v>1</v>
@@ -1905,22 +1911,22 @@
         <v>0</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R12" s="2">
         <v>1</v>
@@ -1958,22 +1964,22 @@
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R13" s="2">
         <v>1</v>
@@ -2011,22 +2017,22 @@
         <v>0</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R14" s="2">
         <v>1</v>
@@ -2064,22 +2070,22 @@
         <v>0</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R15" s="2">
         <v>1</v>
@@ -2117,22 +2123,22 @@
         <v>0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R16" s="2">
         <v>1</v>
@@ -2170,22 +2176,22 @@
         <v>0</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R17" s="2">
         <v>1</v>
@@ -2223,22 +2229,22 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R18" s="2">
         <v>1</v>
@@ -2276,22 +2282,22 @@
         <v>0</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R19" s="2">
         <v>1</v>
@@ -2329,22 +2335,22 @@
         <v>0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R20" s="2">
         <v>1</v>
@@ -2382,22 +2388,22 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R21" s="2">
         <v>1</v>
@@ -2435,22 +2441,22 @@
         <v>0</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R22" s="2">
         <v>1</v>
@@ -2488,22 +2494,22 @@
         <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R23" s="2">
         <v>1</v>
@@ -2541,22 +2547,22 @@
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R24" s="2">
         <v>1</v>
@@ -2594,22 +2600,22 @@
         <v>0</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R25" s="2">
         <v>1</v>
@@ -2647,22 +2653,22 @@
         <v>0</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R26" s="2">
         <v>1</v>
@@ -2700,22 +2706,22 @@
         <v>0</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R27" s="2">
         <v>1</v>
@@ -2753,22 +2759,22 @@
         <v>0</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R28" s="2">
         <v>1</v>
@@ -2806,22 +2812,22 @@
         <v>0</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R29" s="2">
         <v>1</v>
@@ -2859,22 +2865,22 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R30" s="2">
         <v>1</v>
@@ -2912,22 +2918,22 @@
         <v>0</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R31" s="2">
         <v>1</v>
@@ -2965,22 +2971,22 @@
         <v>0</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R32" s="2">
         <v>1</v>
@@ -3018,22 +3024,22 @@
         <v>0</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R33" s="2">
         <v>1</v>
@@ -3071,22 +3077,22 @@
         <v>0</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R34" s="2">
         <v>1</v>
@@ -3124,22 +3130,22 @@
         <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R35" s="2">
         <v>1</v>
@@ -3177,22 +3183,22 @@
         <v>0</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R36" s="2">
         <v>1</v>
@@ -3230,22 +3236,22 @@
         <v>0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R37" s="2">
         <v>1</v>
@@ -3283,22 +3289,22 @@
         <v>50</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R38" s="2">
         <v>1</v>
@@ -3336,22 +3342,22 @@
         <v>82.432432430000006</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R39" s="2">
         <v>1</v>
@@ -3389,22 +3395,22 @@
         <v>100</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R40" s="2">
         <v>1</v>
@@ -3442,22 +3448,22 @@
         <v>42.62295082</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q41" s="4"/>
       <c r="R41" s="2">
@@ -3496,22 +3502,22 @@
         <v>22.826086960000001</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q42" s="4"/>
       <c r="R42" s="2">
@@ -3550,22 +3556,22 @@
         <v>24.324324319999999</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="2">
@@ -3604,22 +3610,22 @@
         <v>16.129032259999999</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q44" s="4"/>
       <c r="R44" s="2">
@@ -3658,22 +3664,22 @@
         <v>44.736842109999998</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q45" s="4"/>
       <c r="R45" s="2">
@@ -3712,22 +3718,22 @@
         <v>100</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q46" s="4"/>
       <c r="R46" s="2">
@@ -3766,22 +3772,22 @@
         <v>18.18181818</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q47" s="4"/>
       <c r="R47" s="2">
@@ -3820,22 +3826,22 @@
         <v>5.9523809520000004</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q48" s="4"/>
       <c r="R48" s="2">
@@ -3874,22 +3880,22 @@
         <v>15.38461538</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R49" s="2">
         <v>1</v>
@@ -3927,22 +3933,22 @@
         <v>0</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R50" s="2">
         <v>1</v>
@@ -3980,22 +3986,22 @@
         <v>0</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L51" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N51" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M51" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N51" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O51" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R51" s="2">
         <v>1</v>
@@ -4033,22 +4039,22 @@
         <v>0</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R52" s="2">
         <v>1</v>
@@ -4086,22 +4092,22 @@
         <v>0</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L53" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N53" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M53" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N53" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O53" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R53" s="2">
         <v>1</v>
@@ -4139,22 +4145,22 @@
         <v>0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R54" s="2">
         <v>1</v>
@@ -4192,22 +4198,22 @@
         <v>0</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L55" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N55" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M55" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O55" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R55" s="2">
         <v>1</v>
@@ -4245,22 +4251,22 @@
         <v>0</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R56" s="2">
         <v>1</v>
@@ -4298,22 +4304,22 @@
         <v>0</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N57" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M57" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O57" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R57" s="2">
         <v>1</v>
@@ -4351,22 +4357,22 @@
         <v>0</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R58" s="2">
         <v>1</v>
@@ -4404,22 +4410,22 @@
         <v>0</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L59" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N59" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M59" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O59" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R59" s="2">
         <v>1</v>
@@ -4457,22 +4463,22 @@
         <v>0</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R60" s="2">
         <v>1</v>
@@ -4510,22 +4516,22 @@
         <v>0</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L61" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N61" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M61" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N61" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O61" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R61" s="2">
         <v>1</v>
@@ -4563,22 +4569,22 @@
         <v>0</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q62" s="2" t="s">
         <v>156</v>
@@ -4619,22 +4625,22 @@
         <v>0</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L63" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N63" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M63" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N63" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O63" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q63" s="2" t="s">
         <v>156</v>
@@ -4675,22 +4681,22 @@
         <v>0</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R64" s="2">
         <v>1</v>
@@ -4728,22 +4734,22 @@
         <v>0</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L65" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N65" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M65" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O65" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R65" s="2">
         <v>1</v>
@@ -4781,22 +4787,22 @@
         <v>0</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R66" s="2">
         <v>1</v>
@@ -4834,22 +4840,22 @@
         <v>0</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L67" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N67" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M67" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N67" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O67" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R67" s="2">
         <v>1</v>
@@ -4887,22 +4893,22 @@
         <v>0</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R68" s="2">
         <v>1</v>
@@ -4940,22 +4946,22 @@
         <v>0</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L69" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N69" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M69" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N69" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O69" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R69" s="2">
         <v>1</v>
@@ -4993,22 +4999,22 @@
         <v>0</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R70" s="2">
         <v>1</v>
@@ -5046,22 +5052,22 @@
         <v>0</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L71" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N71" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M71" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O71" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R71" s="2">
         <v>1</v>
@@ -5099,22 +5105,22 @@
         <v>0</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R72" s="2">
         <v>1</v>
@@ -5152,22 +5158,22 @@
         <v>0</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L73" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N73" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M73" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N73" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O73" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R73" s="2">
         <v>1</v>
@@ -5205,22 +5211,22 @@
         <v>78.947368420000004</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N74" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O74" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O74" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P74" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R74" s="2">
         <v>1</v>
@@ -5258,22 +5264,22 @@
         <v>10.958904110000001</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L75" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N75" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M75" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N75" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O75" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R75" s="2">
         <v>1</v>
@@ -5311,22 +5317,22 @@
         <v>61.53846154</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N76" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O76" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O76" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P76" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R76" s="2">
         <v>1</v>
@@ -5364,22 +5370,22 @@
         <v>27.027027029999999</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L77" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N77" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M77" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N77" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O77" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P77" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R77" s="2">
         <v>1</v>
@@ -5417,22 +5423,22 @@
         <v>58.536585369999997</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N78" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O78" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O78" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P78" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R78" s="2">
         <v>1</v>
@@ -5470,22 +5476,22 @@
         <v>61.111111110000003</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L79" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N79" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M79" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N79" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O79" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R79" s="2">
         <v>1</v>
@@ -5523,22 +5529,22 @@
         <v>0</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P80" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R80" s="2">
         <v>1</v>
@@ -5576,22 +5582,22 @@
         <v>0</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L81" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N81" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M81" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N81" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O81" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R81" s="2">
         <v>1</v>
@@ -5629,22 +5635,22 @@
         <v>30.76923077</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N82" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O82" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O82" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P82" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R82" s="2">
         <v>1</v>
@@ -5682,22 +5688,22 @@
         <v>1.123595506</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L83" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N83" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M83" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N83" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O83" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P83" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R83" s="2">
         <v>1</v>
@@ -5735,22 +5741,22 @@
         <v>18.421052629999998</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N84" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O84" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O84" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P84" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R84" s="2">
         <v>1</v>
@@ -5788,22 +5794,22 @@
         <v>18.75</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L85" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N85" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M85" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N85" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O85" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R85" s="2">
         <v>1</v>
@@ -5841,22 +5847,22 @@
         <v>27.777777780000001</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N86" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O86" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O86" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P86" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R86" s="2">
         <v>1</v>
@@ -5894,22 +5900,22 @@
         <v>21.621621619999999</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L87" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N87" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M87" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N87" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O87" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R87" s="2">
         <v>1</v>
@@ -5947,22 +5953,22 @@
         <v>0</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R88" s="2">
         <v>1</v>
@@ -6000,22 +6006,22 @@
         <v>0</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L89" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N89" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M89" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N89" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O89" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R89" s="2">
         <v>1</v>
@@ -6053,22 +6059,22 @@
         <v>0</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R90" s="2">
         <v>1</v>
@@ -6106,22 +6112,22 @@
         <v>0</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L91" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M91" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N91" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M91" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N91" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O91" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R91" s="2">
         <v>1</v>
@@ -6153,22 +6159,22 @@
       <c r="I92" s="10"/>
       <c r="J92" s="13"/>
       <c r="K92" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M92" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N92" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O92" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O92" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P92" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="Q92" s="2" t="s">
         <v>204</v>
@@ -6203,22 +6209,22 @@
       <c r="I93" s="10"/>
       <c r="J93" s="13"/>
       <c r="K93" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L93" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M93" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N93" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M93" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N93" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O93" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Q93" s="2" t="s">
         <v>204</v>
@@ -6259,22 +6265,22 @@
         <v>11.764705879999999</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N94" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O94" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O94" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P94" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R94" s="2">
         <v>1</v>
@@ -6296,7 +6302,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection activeCell="K1" sqref="K1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6343,22 +6349,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>17</v>
@@ -6399,22 +6405,22 @@
         <v>78.947368420000004</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -6452,22 +6458,22 @@
         <v>10.958904110000001</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O3" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -6505,22 +6511,22 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
@@ -6558,22 +6564,22 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O5" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -6589,8 +6595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6637,22 +6643,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>17</v>
@@ -6693,22 +6699,22 @@
         <v>78.947368420000004</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -6746,22 +6752,22 @@
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Updated by adding log
also changed compression to earlier form
</commit_message>
<xml_diff>
--- a/test_metafile_2boxes.xlsx
+++ b/test_metafile_2boxes.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14145" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14145" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="thph12_metafile" sheetId="1" r:id="rId1"/>
-    <sheet name="test_2boxes" sheetId="3" r:id="rId2"/>
-    <sheet name="test_1box" sheetId="4" r:id="rId3"/>
+    <sheet name="test_metafile_2boxes" sheetId="3" r:id="rId2"/>
+    <sheet name="test_metafile_1box" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="227">
   <si>
     <t>tdtfile</t>
   </si>
@@ -648,9 +648,18 @@
     <t>!2017-08-16_10h52m.Subject THPH2.7</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>uv</t>
+  </si>
+  <si>
     <t>tick</t>
   </si>
   <si>
+    <t>distractors</t>
+  </si>
+  <si>
     <t>Dv1A</t>
   </si>
   <si>
@@ -694,21 +703,6 @@
   </si>
   <si>
     <t>Do2_</t>
-  </si>
-  <si>
-    <t>sig-blue</t>
-  </si>
-  <si>
-    <t>sig-uv</t>
-  </si>
-  <si>
-    <t>ttl-licks</t>
-  </si>
-  <si>
-    <t>ttl-distractors</t>
-  </si>
-  <si>
-    <t>ttl-distracted</t>
   </si>
 </sst>
 </file>
@@ -1277,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P1"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1325,22 +1319,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>228</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>17</v>
@@ -1381,22 +1375,22 @@
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -1434,22 +1428,22 @@
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -1487,22 +1481,22 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
@@ -1540,22 +1534,22 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -1593,22 +1587,22 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
@@ -1646,22 +1640,22 @@
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R7" s="2">
         <v>1</v>
@@ -1699,22 +1693,22 @@
         <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R8" s="2">
         <v>1</v>
@@ -1752,22 +1746,22 @@
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R9" s="2">
         <v>1</v>
@@ -1805,22 +1799,22 @@
         <v>0</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R10" s="2">
         <v>1</v>
@@ -1858,22 +1852,22 @@
         <v>0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R11" s="2">
         <v>1</v>
@@ -1911,22 +1905,22 @@
         <v>0</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R12" s="2">
         <v>1</v>
@@ -1964,22 +1958,22 @@
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R13" s="2">
         <v>1</v>
@@ -2017,22 +2011,22 @@
         <v>0</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R14" s="2">
         <v>1</v>
@@ -2070,22 +2064,22 @@
         <v>0</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R15" s="2">
         <v>1</v>
@@ -2123,22 +2117,22 @@
         <v>0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R16" s="2">
         <v>1</v>
@@ -2176,22 +2170,22 @@
         <v>0</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R17" s="2">
         <v>1</v>
@@ -2229,22 +2223,22 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R18" s="2">
         <v>1</v>
@@ -2282,22 +2276,22 @@
         <v>0</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R19" s="2">
         <v>1</v>
@@ -2335,22 +2329,22 @@
         <v>0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R20" s="2">
         <v>1</v>
@@ -2388,22 +2382,22 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R21" s="2">
         <v>1</v>
@@ -2441,22 +2435,22 @@
         <v>0</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R22" s="2">
         <v>1</v>
@@ -2494,22 +2488,22 @@
         <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R23" s="2">
         <v>1</v>
@@ -2547,22 +2541,22 @@
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R24" s="2">
         <v>1</v>
@@ -2600,22 +2594,22 @@
         <v>0</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R25" s="2">
         <v>1</v>
@@ -2653,22 +2647,22 @@
         <v>0</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R26" s="2">
         <v>1</v>
@@ -2706,22 +2700,22 @@
         <v>0</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R27" s="2">
         <v>1</v>
@@ -2759,22 +2753,22 @@
         <v>0</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R28" s="2">
         <v>1</v>
@@ -2812,22 +2806,22 @@
         <v>0</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R29" s="2">
         <v>1</v>
@@ -2865,22 +2859,22 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R30" s="2">
         <v>1</v>
@@ -2918,22 +2912,22 @@
         <v>0</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R31" s="2">
         <v>1</v>
@@ -2971,22 +2965,22 @@
         <v>0</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R32" s="2">
         <v>1</v>
@@ -3024,22 +3018,22 @@
         <v>0</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R33" s="2">
         <v>1</v>
@@ -3077,22 +3071,22 @@
         <v>0</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R34" s="2">
         <v>1</v>
@@ -3130,22 +3124,22 @@
         <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R35" s="2">
         <v>1</v>
@@ -3183,22 +3177,22 @@
         <v>0</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R36" s="2">
         <v>1</v>
@@ -3236,22 +3230,22 @@
         <v>0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R37" s="2">
         <v>1</v>
@@ -3289,22 +3283,22 @@
         <v>50</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R38" s="2">
         <v>1</v>
@@ -3342,22 +3336,22 @@
         <v>82.432432430000006</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R39" s="2">
         <v>1</v>
@@ -3395,22 +3389,22 @@
         <v>100</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R40" s="2">
         <v>1</v>
@@ -3448,22 +3442,22 @@
         <v>42.62295082</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q41" s="4"/>
       <c r="R41" s="2">
@@ -3502,22 +3496,22 @@
         <v>22.826086960000001</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q42" s="4"/>
       <c r="R42" s="2">
@@ -3556,22 +3550,22 @@
         <v>24.324324319999999</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="2">
@@ -3610,22 +3604,22 @@
         <v>16.129032259999999</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q44" s="4"/>
       <c r="R44" s="2">
@@ -3664,22 +3658,22 @@
         <v>44.736842109999998</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q45" s="4"/>
       <c r="R45" s="2">
@@ -3718,22 +3712,22 @@
         <v>100</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q46" s="4"/>
       <c r="R46" s="2">
@@ -3772,22 +3766,22 @@
         <v>18.18181818</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q47" s="4"/>
       <c r="R47" s="2">
@@ -3826,22 +3820,22 @@
         <v>5.9523809520000004</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q48" s="4"/>
       <c r="R48" s="2">
@@ -3880,22 +3874,22 @@
         <v>15.38461538</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R49" s="2">
         <v>1</v>
@@ -3933,22 +3927,22 @@
         <v>0</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R50" s="2">
         <v>1</v>
@@ -3986,22 +3980,22 @@
         <v>0</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R51" s="2">
         <v>1</v>
@@ -4039,22 +4033,22 @@
         <v>0</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R52" s="2">
         <v>1</v>
@@ -4092,22 +4086,22 @@
         <v>0</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R53" s="2">
         <v>1</v>
@@ -4145,22 +4139,22 @@
         <v>0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R54" s="2">
         <v>1</v>
@@ -4198,22 +4192,22 @@
         <v>0</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R55" s="2">
         <v>1</v>
@@ -4251,22 +4245,22 @@
         <v>0</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R56" s="2">
         <v>1</v>
@@ -4304,22 +4298,22 @@
         <v>0</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R57" s="2">
         <v>1</v>
@@ -4357,22 +4351,22 @@
         <v>0</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R58" s="2">
         <v>1</v>
@@ -4410,22 +4404,22 @@
         <v>0</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R59" s="2">
         <v>1</v>
@@ -4463,22 +4457,22 @@
         <v>0</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R60" s="2">
         <v>1</v>
@@ -4516,22 +4510,22 @@
         <v>0</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R61" s="2">
         <v>1</v>
@@ -4569,22 +4563,22 @@
         <v>0</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q62" s="2" t="s">
         <v>156</v>
@@ -4625,22 +4619,22 @@
         <v>0</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="Q63" s="2" t="s">
         <v>156</v>
@@ -4681,22 +4675,22 @@
         <v>0</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R64" s="2">
         <v>1</v>
@@ -4734,22 +4728,22 @@
         <v>0</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R65" s="2">
         <v>1</v>
@@ -4787,22 +4781,22 @@
         <v>0</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R66" s="2">
         <v>1</v>
@@ -4840,22 +4834,22 @@
         <v>0</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R67" s="2">
         <v>1</v>
@@ -4893,22 +4887,22 @@
         <v>0</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R68" s="2">
         <v>1</v>
@@ -4946,22 +4940,22 @@
         <v>0</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R69" s="2">
         <v>1</v>
@@ -4999,22 +4993,22 @@
         <v>0</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R70" s="2">
         <v>1</v>
@@ -5052,22 +5046,22 @@
         <v>0</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R71" s="2">
         <v>1</v>
@@ -5105,22 +5099,22 @@
         <v>0</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R72" s="2">
         <v>1</v>
@@ -5158,22 +5152,22 @@
         <v>0</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R73" s="2">
         <v>1</v>
@@ -5211,22 +5205,22 @@
         <v>78.947368420000004</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R74" s="2">
         <v>1</v>
@@ -5264,22 +5258,22 @@
         <v>10.958904110000001</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R75" s="2">
         <v>1</v>
@@ -5317,22 +5311,22 @@
         <v>61.53846154</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R76" s="2">
         <v>1</v>
@@ -5370,22 +5364,22 @@
         <v>27.027027029999999</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P77" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R77" s="2">
         <v>1</v>
@@ -5423,22 +5417,22 @@
         <v>58.536585369999997</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P78" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R78" s="2">
         <v>1</v>
@@ -5476,22 +5470,22 @@
         <v>61.111111110000003</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R79" s="2">
         <v>1</v>
@@ -5529,22 +5523,22 @@
         <v>0</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P80" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R80" s="2">
         <v>1</v>
@@ -5582,22 +5576,22 @@
         <v>0</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R81" s="2">
         <v>1</v>
@@ -5635,22 +5629,22 @@
         <v>30.76923077</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R82" s="2">
         <v>1</v>
@@ -5688,22 +5682,22 @@
         <v>1.123595506</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P83" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R83" s="2">
         <v>1</v>
@@ -5741,22 +5735,22 @@
         <v>18.421052629999998</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P84" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R84" s="2">
         <v>1</v>
@@ -5794,22 +5788,22 @@
         <v>18.75</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R85" s="2">
         <v>1</v>
@@ -5847,22 +5841,22 @@
         <v>27.777777780000001</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R86" s="2">
         <v>1</v>
@@ -5900,22 +5894,22 @@
         <v>21.621621619999999</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R87" s="2">
         <v>1</v>
@@ -5953,22 +5947,22 @@
         <v>0</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R88" s="2">
         <v>1</v>
@@ -6006,22 +6000,22 @@
         <v>0</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R89" s="2">
         <v>1</v>
@@ -6059,22 +6053,22 @@
         <v>0</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R90" s="2">
         <v>1</v>
@@ -6112,22 +6106,22 @@
         <v>0</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R91" s="2">
         <v>1</v>
@@ -6159,22 +6153,22 @@
       <c r="I92" s="10"/>
       <c r="J92" s="13"/>
       <c r="K92" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M92" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O92" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="Q92" s="2" t="s">
         <v>204</v>
@@ -6209,22 +6203,22 @@
       <c r="I93" s="10"/>
       <c r="J93" s="13"/>
       <c r="K93" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M93" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O93" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="Q93" s="2" t="s">
         <v>204</v>
@@ -6265,22 +6259,22 @@
         <v>11.764705879999999</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P94" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R94" s="2">
         <v>1</v>
@@ -6301,8 +6295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6349,22 +6343,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>228</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>17</v>
@@ -6405,22 +6399,22 @@
         <v>78.947368420000004</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -6458,22 +6452,22 @@
         <v>10.958904110000001</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -6511,22 +6505,22 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
@@ -6564,22 +6558,22 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -6596,7 +6590,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6643,22 +6637,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>228</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>17</v>
@@ -6699,22 +6693,22 @@
         <v>78.947368420000004</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -6752,22 +6746,22 @@
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>

</xml_diff>